<commit_message>
status: finish turn PM
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="estudos" sheetId="1" r:id="rId1"/>
+    <sheet name="Estudos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>DATA</t>
   </si>
@@ -31,10 +31,16 @@
     <t>HORA F</t>
   </si>
   <si>
-    <t>Aula de HARD (Controle de sessão) + Início de implemetação do controle de produtos o projeto green_collections</t>
-  </si>
-  <si>
     <t>HARD</t>
+  </si>
+  <si>
+    <t>DESCANSO</t>
+  </si>
+  <si>
+    <t>Aula de HARD (Controle de sessão) + Início de implemetação do controle de produtos o (projeto green collections)</t>
+  </si>
+  <si>
+    <t>Implementação de controle de produtos (projeto green collections) + Ajuda alpha (Atividade extra)</t>
   </si>
 </sst>
 </file>
@@ -101,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -121,9 +127,6 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -131,7 +134,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -272,14 +294,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:E3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E3"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="DATA" dataDxfId="4"/>
-    <tableColumn id="2" name="HORA I" dataDxfId="3"/>
-    <tableColumn id="3" name="HORA F" dataDxfId="2"/>
-    <tableColumn id="4" name="ASSUNTO" dataDxfId="1"/>
-    <tableColumn id="5" name="PRODUÇÃO" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F3" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F3"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="DATA" dataDxfId="5"/>
+    <tableColumn id="2" name="HORA I" dataDxfId="4"/>
+    <tableColumn id="3" name="HORA F" dataDxfId="3"/>
+    <tableColumn id="4" name="ASSUNTO" dataDxfId="2"/>
+    <tableColumn id="5" name="PRODUÇÃO" dataDxfId="1"/>
+    <tableColumn id="6" name="DESCANSO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -572,23 +595,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="22" style="1" customWidth="1"/>
     <col min="5" max="5" width="59.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="12.140625" style="1"/>
+    <col min="6" max="6" width="59.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="12.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -604,8 +628,11 @@
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44837</v>
       </c>
@@ -616,22 +643,34 @@
         <v>0.50624999999999998</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44837</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="3">
         <v>0.58819444444444446</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="3">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0416666666666666E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
status: end turn AM
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>DATA</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Implementação de controle de produtos (projeto green collections) + Ajuda alpha (Atividade extra)</t>
+  </si>
+  <si>
+    <t>Aula de HARD (Criptografia) + implemetação do controle de produtos o (projeto green collections)</t>
   </si>
 </sst>
 </file>
@@ -297,8 +300,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F5"/>
   <tableColumns count="6">
     <tableColumn id="1" name="DATA" dataDxfId="5"/>
     <tableColumn id="2" name="HORA I" dataDxfId="4"/>
@@ -598,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -675,17 +678,35 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44838</v>
       </c>
       <c r="B4" s="8">
         <v>0.3923611111111111</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="8">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>44838</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
status: init work noturn
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>DATA</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t>Implementação de controle de produtos (projeto green collections) + Ajuda alpha (Atividade extra)</t>
+  </si>
+  <si>
+    <t>Aula de HARD (Criptografia) +  implemetação do controle de produtos o (projeto green collections)</t>
+  </si>
+  <si>
+    <t>Momento empresa (feedback) + implementação de produtos (projeto green collections)</t>
+  </si>
+  <si>
+    <t>Implementação de produtos green collections</t>
   </si>
 </sst>
 </file>
@@ -297,8 +306,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F6"/>
   <tableColumns count="6">
     <tableColumn id="1" name="DATA" dataDxfId="5"/>
     <tableColumn id="2" name="HORA I" dataDxfId="4"/>
@@ -598,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -675,17 +684,61 @@
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44838</v>
       </c>
       <c r="B4" s="8">
         <v>0.3923611111111111</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="8">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1.0416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>44838</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.58194444444444449</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.79722222222222217</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>44838</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.85763888888888884</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
status: finish work 04/10/2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -610,7 +610,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -731,14 +731,18 @@
       <c r="B6" s="8">
         <v>0.85763888888888884</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8">
+        <v>0.91319444444444453</v>
+      </c>
       <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
status: init work 05_10
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -306,8 +306,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F7"/>
   <tableColumns count="6">
     <tableColumn id="1" name="DATA" dataDxfId="5"/>
     <tableColumn id="2" name="HORA I" dataDxfId="4"/>
@@ -607,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -744,6 +744,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>44839</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
status: init work PM
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Estudos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>DATA</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Aula de HARD (JWT) +  implemetação produtos do projeto green collections</t>
+  </si>
+  <si>
+    <t>DIF</t>
   </si>
 </sst>
 </file>
@@ -149,7 +152,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -309,15 +331,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F7"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="DATA" dataDxfId="5"/>
-    <tableColumn id="2" name="HORA I" dataDxfId="4"/>
-    <tableColumn id="3" name="HORA F" dataDxfId="3"/>
-    <tableColumn id="4" name="ASSUNTO" dataDxfId="2"/>
-    <tableColumn id="5" name="PRODUÇÃO" dataDxfId="1"/>
-    <tableColumn id="6" name="DESCANSO" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G8" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G8"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="DATA" dataDxfId="6"/>
+    <tableColumn id="2" name="HORA I" dataDxfId="5"/>
+    <tableColumn id="3" name="HORA F" dataDxfId="4"/>
+    <tableColumn id="8" name="DIF" dataDxfId="0">
+      <calculatedColumnFormula>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="ASSUNTO" dataDxfId="3"/>
+    <tableColumn id="5" name="PRODUÇÃO" dataDxfId="2"/>
+    <tableColumn id="6" name="DESCANSO" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -610,24 +635,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22" style="1" customWidth="1"/>
-    <col min="5" max="5" width="59.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="59.85546875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="12.140625" style="1"/>
+    <col min="2" max="2" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="59.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="5" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -638,16 +664,19 @@
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44837</v>
       </c>
@@ -657,17 +686,21 @@
       <c r="C2" s="3">
         <v>0.50624999999999998</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>0.17152777777777778</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44837</v>
       </c>
@@ -677,17 +710,21 @@
       <c r="C3" s="3">
         <v>0.76736111111111116</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>0.1791666666666667</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44838</v>
       </c>
@@ -697,17 +734,21 @@
       <c r="C4" s="8">
         <v>0.47916666666666669</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>8.680555555555558E-2</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G4" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>44838</v>
       </c>
@@ -717,17 +758,21 @@
       <c r="C5" s="8">
         <v>0.79722222222222217</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="3">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>0.21527777777777768</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8">
+      <c r="G5" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>44838</v>
       </c>
@@ -737,17 +782,21 @@
       <c r="C6" s="8">
         <v>0.91319444444444453</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="3">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>5.5555555555555691E-2</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G6" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>44839</v>
       </c>
@@ -757,15 +806,33 @@
       <c r="C7" s="8">
         <v>0.54861111111111105</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="3">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>0.18055555555555547</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G7" s="8">
         <v>1.0416666666666666E-2</v>
       </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="8">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="3">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>-0.59722222222222221</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
status: init work AM
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -334,8 +334,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G10"/>
   <tableColumns count="7">
     <tableColumn id="1" name="DATA" dataDxfId="6"/>
     <tableColumn id="2" name="HORA I" dataDxfId="5"/>
@@ -638,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -867,6 +867,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="8">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>-0.3923611111111111</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
date: 11 10 2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
   <si>
     <t>DATA</t>
   </si>
@@ -346,8 +346,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G17" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G17"/>
   <tableColumns count="7">
     <tableColumn id="1" name="DATA" dataDxfId="6"/>
     <tableColumn id="2" name="HORA I" dataDxfId="5"/>
@@ -650,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1051,6 +1051,30 @@
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>44844</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1.2486111111111111</v>
+      </c>
+      <c r="D17" s="8">
+        <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
+        <v>0.99861111111111112</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="8">
+        <v>2.7777777777777776E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
chore: init work 31
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="35">
   <si>
     <t>DATA</t>
   </si>
@@ -76,9 +76,6 @@
     <t>ÚTEIS</t>
   </si>
   <si>
-    <t>Implementação de projeto plant collections + atividade voluntária no Alpha EdTeck</t>
-  </si>
-  <si>
     <t>Implementação de projeto plant collections + apresentação de andamento do projeto</t>
   </si>
   <si>
@@ -88,31 +85,40 @@
     <t>Finalização e apresentação do projero green gollections</t>
   </si>
   <si>
-    <t>Atividade voluntária no Alpha EdTeck + Curso de segurança da informação</t>
-  </si>
-  <si>
-    <t>Atividade voluntária no Alpha EdTeck + revisão de javascript</t>
-  </si>
-  <si>
-    <t>Atividade voluntária no Alpha EdTeck + resolução de atividades pendentes</t>
-  </si>
-  <si>
-    <t>Atividade voluntária no Alpha EdTeck + Aula de Soft + resolução de atividades pendentes</t>
-  </si>
-  <si>
-    <t>Atividade voluntária no Alpha EdTeck + Typescript</t>
-  </si>
-  <si>
-    <t>Atividade voluntária no Alpha EdTeck</t>
-  </si>
-  <si>
-    <t>Atividade voluntária no Alpha EdTeck + Typescript + Ingles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resolução de atvividades Typescript (TS) + Atividade voluntária no Alpha EdTeck </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atividade voluntária no Alpha EdTeck </t>
+    <t xml:space="preserve">ESTÁGIO + </t>
+  </si>
+  <si>
+    <t>Implementação de projeto plant collections + atividade voluntária no Alpha EdTech</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + Curso de segurança da informação</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + revisão de javascript</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + resolução de atividades pendentes</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + Aula de Soft + resolução de atividades pendentes</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + Typescript</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + Typescript + Ingles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resolução de atvividades Typescript (TS) + Atividade voluntária no Alpha EdTech </t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + Estudando typscript</t>
+  </si>
+  <si>
+    <t>Atividade voluntária no Alpha EdTech + Estágio</t>
   </si>
 </sst>
 </file>
@@ -882,7 +888,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1375,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1397,7 +1403,7 @@
         <v>5</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1537,7 +1543,7 @@
         <v>5</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1562,10 +1568,10 @@
         <v>0</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1590,10 +1596,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1621,7 +1627,7 @@
         <v>5</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1649,7 +1655,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1677,7 +1683,7 @@
         <v>5</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1705,7 +1711,7 @@
         <v>17</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1733,7 +1739,7 @@
         <v>16</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1761,7 +1767,7 @@
         <v>5</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1789,7 +1795,7 @@
         <v>5</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1817,7 +1823,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1873,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1901,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1929,7 +1935,7 @@
         <v>16</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -1957,7 +1963,7 @@
         <v>5</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1967,38 +1973,50 @@
       <c r="B39" s="5">
         <v>0.27083333333333331</v>
       </c>
-      <c r="C39" s="5"/>
+      <c r="C39" s="5">
+        <v>0.5</v>
+      </c>
       <c r="D39" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.27083333333333331</v>
-      </c>
-      <c r="E39" s="5"/>
+        <v>0.22916666666666669</v>
+      </c>
+      <c r="E39" s="5">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F39" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>-0.27083333333333331</v>
-      </c>
-      <c r="G39" s="4"/>
+        <v>0.18750000000000003</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H39" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>44865</v>
       </c>
-      <c r="B40" s="5"/>
+      <c r="B40" s="5">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.33333333333333331</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
+        <v>-0.33333333333333331</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: initi word 06 11 2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>DATA</t>
   </si>
@@ -133,7 +133,7 @@
     <t>Atividade voluntária no Alpha EdTech + InglÊs + Hard</t>
   </si>
   <si>
-    <t>Resolução de atvividades Javascript (JS)</t>
+    <t>Resolução de atividades banco de dados</t>
   </si>
 </sst>
 </file>
@@ -903,7 +903,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="H52" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2156,17 +2156,23 @@
       <c r="B45" s="5">
         <v>0.54861111111111105</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="5">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D45" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.54861111111111105</v>
-      </c>
-      <c r="E45" s="5"/>
+        <v>0.11805555555555558</v>
+      </c>
+      <c r="E45" s="5">
+        <v>6.9444444444444441E-3</v>
+      </c>
       <c r="F45" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>-0.54861111111111105</v>
-      </c>
-      <c r="G45" s="4"/>
+        <v>0.11111111111111113</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H45" s="4" t="s">
         <v>39</v>
       </c>
@@ -2175,19 +2181,25 @@
       <c r="A46" s="9">
         <v>44871</v>
       </c>
-      <c r="B46" s="5"/>
+      <c r="B46" s="5">
+        <v>0.40277777777777773</v>
+      </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.40277777777777773</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>0</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
+        <v>-0.40277777777777773</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="9">

</xml_diff>

<commit_message>
chore: init work 07 11 2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="41">
   <si>
     <t>DATA</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Resolução de atividades banco de dados</t>
+  </si>
+  <si>
+    <t>Estágio</t>
   </si>
 </sst>
 </file>
@@ -902,8 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2184,15 +2187,19 @@
       <c r="B46" s="5">
         <v>0.40277777777777773</v>
       </c>
-      <c r="C46" s="5"/>
+      <c r="C46" s="5">
+        <v>0.75</v>
+      </c>
       <c r="D46" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.40277777777777773</v>
-      </c>
-      <c r="E46" s="5"/>
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E46" s="5">
+        <v>6.25E-2</v>
+      </c>
       <c r="F46" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>-0.40277777777777773</v>
+        <v>0.28472222222222227</v>
       </c>
       <c r="G46" s="4" t="s">
         <v>5</v>
@@ -2205,19 +2212,23 @@
       <c r="A47" s="9">
         <v>44872</v>
       </c>
-      <c r="B47" s="5"/>
+      <c r="B47" s="5">
+        <v>0.35416666666666669</v>
+      </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.35416666666666669</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>0</v>
+        <v>-0.35416666666666669</v>
       </c>
       <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
+      <c r="H47" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="9">

</xml_diff>

<commit_message>
chore: end wrod 18 and init work 19
init work day 18, 11, 2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
   <si>
     <t>DATA</t>
   </si>
@@ -163,7 +163,7 @@
     <t>Estágio + HARD + SOFT + Atividade voluntária no Alpha EdTech</t>
   </si>
   <si>
-    <t>Estágio</t>
+    <t>Estágio + HARD + INGLÊS</t>
   </si>
 </sst>
 </file>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2550,15 +2550,19 @@
       <c r="B58" s="5">
         <v>0.28819444444444448</v>
       </c>
-      <c r="C58" s="5"/>
+      <c r="C58" s="5">
+        <v>0.84930555555555554</v>
+      </c>
       <c r="D58" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.28819444444444448</v>
-      </c>
-      <c r="E58" s="5"/>
+        <v>0.56111111111111112</v>
+      </c>
+      <c r="E58" s="5">
+        <v>0.18680555555555556</v>
+      </c>
       <c r="F58" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>-0.28819444444444448</v>
+        <v>0.37430555555555556</v>
       </c>
       <c r="G58" s="4" t="s">
         <v>35</v>
@@ -2571,19 +2575,23 @@
       <c r="A59" s="9">
         <v>44884</v>
       </c>
-      <c r="B59" s="5"/>
+      <c r="B59" s="5">
+        <v>0.71180555555555547</v>
+      </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.71180555555555547</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>0</v>
+        <v>-0.71180555555555547</v>
       </c>
       <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
+      <c r="H59" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="9">

</xml_diff>

<commit_message>
chore: init the work
init the work day 22_11_2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
   <si>
     <t>DATA</t>
   </si>
@@ -936,7 +936,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2660,18 +2660,22 @@
       <c r="A62" s="9">
         <v>44887</v>
       </c>
-      <c r="B62" s="5"/>
+      <c r="B62" s="5">
+        <v>0.3125</v>
+      </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.3125</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>0</v>
-      </c>
-      <c r="G62" s="4"/>
+        <v>-0.3125</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="H62" s="4"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
chore: end of work
end of work on day 22,11,2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="51">
   <si>
     <t>DATA</t>
   </si>
@@ -2663,20 +2663,26 @@
       <c r="B62" s="5">
         <v>0.3125</v>
       </c>
-      <c r="C62" s="5"/>
+      <c r="C62" s="5">
+        <v>0.80555555555555547</v>
+      </c>
       <c r="D62" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.3125</v>
-      </c>
-      <c r="E62" s="5"/>
+        <v>0.49305555555555547</v>
+      </c>
+      <c r="E62" s="5">
+        <v>0.12361111111111112</v>
+      </c>
       <c r="F62" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>-0.3125</v>
+        <v>0.36944444444444435</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H62" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="9">

</xml_diff>

<commit_message>
chore: init of work
init of work on day 23, 11, 2022
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
   <si>
     <t>DATA</t>
   </si>
@@ -936,7 +936,7 @@
   <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2688,19 +2688,25 @@
       <c r="A63" s="9">
         <v>44888</v>
       </c>
-      <c r="B63" s="5"/>
+      <c r="B63" s="5">
+        <v>0.3263888888888889</v>
+      </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.3263888888888889</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[DESCANSO]]</f>
-        <v>0</v>
-      </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
+        <v>-0.3263888888888889</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="9">

</xml_diff>

<commit_message>
chore: end and init work
end work day 29 and init work on day 30
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="54">
   <si>
     <t>DATA</t>
   </si>
@@ -945,7 +945,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2860,18 +2860,22 @@
       <c r="B69" s="5">
         <v>0.3125</v>
       </c>
-      <c r="C69" s="5"/>
+      <c r="C69" s="5">
+        <v>0.6875</v>
+      </c>
       <c r="D69" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.3125</v>
-      </c>
-      <c r="E69" s="5"/>
+        <v>0.375</v>
+      </c>
+      <c r="E69" s="5">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="F69" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[PAUSAS]]</f>
-        <v>-0.3125</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H69" s="4" t="s">
         <v>51</v>
@@ -2881,19 +2885,25 @@
       <c r="A70" s="9">
         <v>44895</v>
       </c>
-      <c r="B70" s="5"/>
+      <c r="B70" s="5">
+        <v>0.61111111111111105</v>
+      </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.61111111111111105</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[PAUSAS]]</f>
-        <v>0</v>
-      </c>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
+        <v>-0.61111111111111105</v>
+      </c>
+      <c r="G70" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="9">

</xml_diff>

<commit_message>
chore: end work and init work
end work on day 01 and initt work on day 02
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
   <si>
     <t>DATA</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t xml:space="preserve">Estágio + Atividade voluntária no Alpha EdTech </t>
+  </si>
+  <si>
+    <t>ESTÁGIO + HARD + SOFT</t>
+  </si>
+  <si>
+    <t>Estágio + Hard + Soft</t>
   </si>
 </sst>
 </file>
@@ -945,7 +951,7 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2909,47 +2915,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>44896</v>
       </c>
       <c r="B71" s="5">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C71" s="5"/>
+      <c r="C71" s="5">
+        <v>0.75</v>
+      </c>
       <c r="D71" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.29166666666666669</v>
-      </c>
-      <c r="E71" s="5"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E71" s="5">
+        <v>0.20138888888888887</v>
+      </c>
       <c r="F71" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[PAUSAS]]</f>
-        <v>-0.29166666666666669</v>
+        <v>0.25694444444444442</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>44897</v>
       </c>
-      <c r="B72" s="5"/>
+      <c r="B72" s="5">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
+        <v>-0.29166666666666669</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[PAUSAS]]</f>
-        <v>0</v>
-      </c>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
+        <v>-0.29166666666666669</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9">

</xml_diff>

<commit_message>
chore: init and end work
end work on day 04 and work on day 04
</commit_message>
<xml_diff>
--- a/studies.xlsx
+++ b/studies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="58">
   <si>
     <t>DATA</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Estágio + Hard + Soft</t>
+  </si>
+  <si>
+    <t>Estágio + Hard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hard + Atividade voluntária no Alpha EdTech </t>
   </si>
 </sst>
 </file>
@@ -950,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2950,29 +2956,37 @@
       <c r="B72" s="5">
         <v>0.29166666666666669</v>
       </c>
-      <c r="C72" s="5"/>
+      <c r="C72" s="5">
+        <v>0.625</v>
+      </c>
       <c r="D72" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>-0.29166666666666669</v>
-      </c>
-      <c r="E72" s="5"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E72" s="5">
+        <v>0.12222222222222223</v>
+      </c>
       <c r="F72" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[PAUSAS]]</f>
-        <v>-0.29166666666666669</v>
+        <v>0.21111111111111108</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>44898</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="B73" s="5">
+        <v>0</v>
+      </c>
+      <c r="C73" s="5">
+        <v>0</v>
+      </c>
       <c r="D73" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
         <v>0</v>
@@ -2989,19 +3003,29 @@
       <c r="A74" s="9">
         <v>44899</v>
       </c>
-      <c r="B74" s="5"/>
-      <c r="C74" s="5"/>
+      <c r="B74" s="5">
+        <v>0.625</v>
+      </c>
+      <c r="C74" s="5">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="D74" s="5">
         <f>Tabela1[[#This Row],[HORA F]]-Tabela1[[#This Row],[HORA I]]</f>
-        <v>0</v>
-      </c>
-      <c r="E74" s="5"/>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="E74" s="5">
+        <v>9.2361111111111116E-2</v>
+      </c>
       <c r="F74" s="11">
         <f>Tabela1[[#This Row],[DIF]]-Tabela1[[#This Row],[PAUSAS]]</f>
-        <v>0</v>
-      </c>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
+        <v>0.19930555555555551</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="9">

</xml_diff>